<commit_message>
footer add sum of amount and net_weight
</commit_message>
<xml_diff>
--- a/3.xlsx
+++ b/3.xlsx
@@ -1,247 +1,202 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="24750" windowHeight="12080"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="24750" windowHeight="12080" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="报关单" sheetId="3" r:id="rId1"/>
+    <sheet name="报关单" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">报关单!$A$1:$O$2</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'报关单'!$A$1:$O$2</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>总净重：</t>
-  </si>
-  <si>
-    <t>总货值</t>
-  </si>
-  <si>
-    <t>报关人员  
-申报单位</t>
-  </si>
-  <si>
-    <t>报关人员证号</t>
-  </si>
-  <si>
-    <t>电话</t>
-  </si>
-  <si>
-    <t>兹申明对以上内容承担如实申报、依法纳税之法律责任                                         申报单位（签章）</t>
-  </si>
-  <si>
-    <t>海关批注及签章</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="9">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="[$-10804]0.00"/>
-    <numFmt numFmtId="177" formatCode="_([$€-2]* #,##0.00_);_([$€-2]* \(#,##0.00\);_([$€-2]* &quot;-&quot;??_)"/>
-    <numFmt numFmtId="178" formatCode="&quot;US$&quot;#,##0.00_);[Red]\(&quot;US$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="179" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="180" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="5">
+    <numFmt numFmtId="164" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="165" formatCode="_([$€-2]* #,##0.00_);_([$€-2]* \(#,##0.00\);_([$€-2]* &quot;-&quot;??_)"/>
+    <numFmt numFmtId="166" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="[$-10804]0.00"/>
+    <numFmt numFmtId="168" formatCode="&quot;US$&quot;#,##0.00_);[Red]\(&quot;US$&quot;#,##0.00\)"/>
   </numFmts>
   <fonts count="23">
     <font>
-      <sz val="11"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <color indexed="8"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
       <name val="微软雅黑"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
+      <sz val="10"/>
+    </font>
+    <font>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
       <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
       <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
       <sz val="18"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <i val="1"/>
+      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <b val="1"/>
       <color theme="3"/>
+      <sz val="15"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
+      <b val="1"/>
       <color theme="3"/>
+      <sz val="13"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
+      <b val="1"/>
       <color theme="3"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF9C0006"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color theme="0"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
-      <name val="宋体"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="33">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -603,214 +558,232 @@
     </border>
   </borders>
   <cellStyleXfs count="54">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="10" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="11" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="10" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="12" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+  <cellXfs count="24">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="52" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="52">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="52">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -870,19 +843,8 @@
     <cellStyle name="常规 14" xfId="52"/>
     <cellStyle name="常规 2" xfId="53"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
-  <colors>
-    <mruColors>
-      <color rgb="00FF0000"/>
-      <color rgb="00FFFF00"/>
-      <color rgb="00E6B8B7"/>
-    </mruColors>
-  </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors/>
 </styleSheet>
 </file>
 
@@ -1213,8 +1175,9 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName="Sheet1">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P2"/>
@@ -1223,86 +1186,104 @@
       <selection activeCell="A1" sqref="$A1:$XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="5.09090909090909" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.2545454545455" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1272727272727" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5636363636364" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1272727272727" style="1" customWidth="1"/>
-    <col min="6" max="6" width="45.4272727272727" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.2272727272727" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.1090909090909" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1272727272727" style="1" customWidth="1"/>
-    <col min="12" max="13" width="13.8727272727273" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11.3727272727273" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.2545454545455" style="2" customWidth="1"/>
-    <col min="17" max="16384" width="9" style="1"/>
+    <col width="5.09090909090909" customWidth="1" style="1" min="1" max="1"/>
+    <col width="15.2545454545455" customWidth="1" style="1" min="2" max="2"/>
+    <col width="14.1272727272727" customWidth="1" style="1" min="3" max="3"/>
+    <col hidden="1" width="14.5636363636364" customWidth="1" style="1" min="4" max="4"/>
+    <col width="20.1272727272727" customWidth="1" style="1" min="5" max="5"/>
+    <col width="45.4272727272727" customWidth="1" style="1" min="6" max="6"/>
+    <col width="9" customWidth="1" style="1" min="7" max="7"/>
+    <col width="14.5" customWidth="1" style="1" min="8" max="8"/>
+    <col width="11.2272727272727" customWidth="1" style="1" min="9" max="9"/>
+    <col width="10.1090909090909" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.1272727272727" customWidth="1" style="1" min="11" max="11"/>
+    <col width="13.8727272727273" customWidth="1" style="1" min="12" max="13"/>
+    <col width="11.3727272727273" customWidth="1" style="1" min="14" max="14"/>
+    <col width="12.5" customWidth="1" style="1" min="15" max="15"/>
+    <col width="12.2545454545455" customWidth="1" style="16" min="16" max="16"/>
+    <col width="9" customWidth="1" style="1" min="17" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30" customHeight="1" spans="1:16">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11" t="s">
-        <v>0</v>
+    <row r="1" ht="30" customHeight="1" s="17">
+      <c r="A1" s="3" t="n"/>
+      <c r="B1" s="5" t="n"/>
+      <c r="C1" s="5" t="n"/>
+      <c r="D1" s="6" t="n"/>
+      <c r="E1" s="6" t="n"/>
+      <c r="F1" s="6" t="n"/>
+      <c r="G1" s="5" t="n"/>
+      <c r="H1" s="18" t="n"/>
+      <c r="I1" s="19" t="n"/>
+      <c r="J1" s="11" t="n"/>
+      <c r="K1" s="11" t="inlineStr">
+        <is>
+          <t>总净重：</t>
+        </is>
       </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11" t="s">
-        <v>1</v>
+      <c r="L1" s="11" t="n">
+        <v>3156.66</v>
       </c>
-      <c r="N1" s="11"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="13"/>
+      <c r="M1" s="11" t="inlineStr">
+        <is>
+          <t>总货值</t>
+        </is>
+      </c>
+      <c r="N1" s="11" t="n">
+        <v>29628.36</v>
+      </c>
+      <c r="O1" s="12" t="n"/>
+      <c r="P1" s="20" t="n"/>
     </row>
-    <row r="2" ht="51.95" customHeight="1" spans="1:16">
-      <c r="A2" s="8" t="s">
-        <v>2</v>
+    <row r="2" ht="51.95" customHeight="1" s="17">
+      <c r="A2" s="8" t="inlineStr">
+        <is>
+          <t>报关人员  
+申报单位</t>
+        </is>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9" t="s">
-        <v>3</v>
+      <c r="B2" s="21" t="n"/>
+      <c r="C2" s="21" t="n"/>
+      <c r="D2" s="9" t="inlineStr">
+        <is>
+          <t>报关人员证号</t>
+        </is>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9" t="s">
-        <v>4</v>
+      <c r="E2" s="21" t="n"/>
+      <c r="F2" s="21" t="n"/>
+      <c r="G2" s="21" t="n"/>
+      <c r="H2" s="21" t="n"/>
+      <c r="I2" s="9" t="inlineStr">
+        <is>
+          <t>电话</t>
+        </is>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9" t="s">
-        <v>5</v>
+      <c r="J2" s="21" t="n"/>
+      <c r="K2" s="9" t="inlineStr">
+        <is>
+          <t>兹申明对以上内容承担如实申报、依法纳税之法律责任                                         申报单位（签章）</t>
+        </is>
       </c>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9" t="s">
-        <v>6</v>
+      <c r="L2" s="21" t="n"/>
+      <c r="M2" s="14" t="inlineStr">
+        <is>
+          <t>海关批注及签章</t>
+        </is>
       </c>
-      <c r="N2" s="9"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="15"/>
+      <c r="N2" s="21" t="n"/>
+      <c r="O2" s="22" t="n"/>
+      <c r="P2" s="23" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="M2:O2"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:O2"/>
   </mergeCells>
   <pageMargins left="0.751388888888889" right="0.751388888888889" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <pageSetup paperSize="9" scale="63" fitToHeight="0" orientation="landscape" horizontalDpi="600"/>
-  <headerFooter/>
+  <pageSetup orientation="landscape" paperSize="9" scale="63" fitToHeight="0" horizontalDpi="600"/>
 </worksheet>
 </file>
</xml_diff>